<commit_message>
added ASM version of quicksort, SIMD merge sort.
added ASM version of quicksort, SIMD merge sort.
</commit_message>
<xml_diff>
--- a/test_sorting_algorithms/Sorting_algo.xlsx
+++ b/test_sorting_algorithms/Sorting_algo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>bubble_sort</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>Cpp_sort</t>
+  </si>
+  <si>
+    <t>quick_sort_asm</t>
+  </si>
+  <si>
+    <t>merge</t>
+  </si>
+  <si>
+    <t>merge SIMD</t>
   </si>
 </sst>
 </file>
@@ -336,6 +345,120 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>quick_sort_asm</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$H$4:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>152795</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>322048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>709481</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1523882</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3260794</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6935903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>merge</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$I$4:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>253119</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>564616</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1176012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2512643</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5370808</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11389394</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>merge SIMD</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$J$4:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>107264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>233646</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>528261</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1170422</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2547213</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5542110</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -346,11 +469,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101370880"/>
-        <c:axId val="74684032"/>
+        <c:axId val="107739648"/>
+        <c:axId val="99194496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101370880"/>
+        <c:axId val="107739648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,7 +482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74684032"/>
+        <c:crossAx val="99194496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -367,7 +490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74684032"/>
+        <c:axId val="99194496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -378,7 +501,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101370880"/>
+        <c:crossAx val="107739648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -410,10 +533,10 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -722,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G9"/>
+  <dimension ref="A3:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,9 +858,11 @@
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -756,8 +881,17 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1024</v>
       </c>
@@ -779,8 +913,17 @@
       <c r="G4">
         <v>177976</v>
       </c>
+      <c r="H4">
+        <v>152795</v>
+      </c>
+      <c r="I4">
+        <v>253119</v>
+      </c>
+      <c r="J4">
+        <v>107264</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4*2</f>
         <v>2048</v>
@@ -803,8 +946,17 @@
       <c r="G5">
         <v>390942</v>
       </c>
+      <c r="H5">
+        <v>322048</v>
+      </c>
+      <c r="I5">
+        <v>564616</v>
+      </c>
+      <c r="J5">
+        <v>233646</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ref="A6:A8" si="0">A5*2</f>
         <v>4096</v>
@@ -827,8 +979,17 @@
       <c r="G6">
         <v>858999</v>
       </c>
+      <c r="H6">
+        <v>709481</v>
+      </c>
+      <c r="I6">
+        <v>1176012</v>
+      </c>
+      <c r="J6">
+        <v>528261</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>8192</v>
@@ -851,8 +1012,17 @@
       <c r="G7">
         <v>1847253</v>
       </c>
+      <c r="H7">
+        <v>1523882</v>
+      </c>
+      <c r="I7">
+        <v>2512643</v>
+      </c>
+      <c r="J7">
+        <v>1170422</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>16384</v>
@@ -875,8 +1045,17 @@
       <c r="G8">
         <v>3962942</v>
       </c>
+      <c r="H8">
+        <v>3260794</v>
+      </c>
+      <c r="I8">
+        <v>5370808</v>
+      </c>
+      <c r="J8">
+        <v>2547213</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>33522599</v>
       </c>
@@ -891,6 +1070,15 @@
       </c>
       <c r="G9">
         <v>8496524</v>
+      </c>
+      <c r="H9">
+        <v>6935903</v>
+      </c>
+      <c r="I9">
+        <v>11389394</v>
+      </c>
+      <c r="J9">
+        <v>5542110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>